<commit_message>
Name has changed of project
</commit_message>
<xml_diff>
--- a/Resource/Endpoints.xlsx
+++ b/Resource/Endpoints.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Workspace\projectwork\RestAssuredFrameworkRS\Resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE272E4E-E8AE-4E01-9769-B8873B4FBD8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0074F720-3E7D-4CC6-A1FA-A04FF50B2386}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Base URIs" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="SSL" sheetId="5" r:id="rId3"/>
     <sheet name="Description" sheetId="2" r:id="rId4"/>
     <sheet name="RealTime Steps" sheetId="3" r:id="rId5"/>
+    <sheet name="Query Parameter" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -755,6 +756,72 @@
         <a:xfrm>
           <a:off x="0" y="15592425"/>
           <a:ext cx="8353425" cy="5273747"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>373380</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED8BEA04-2EC6-434C-A359-4D0B45FA4A13}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7078980" cy="1478280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1041,7 +1108,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -1253,7 +1320,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C3494C2-A7A2-4537-833D-C720AA382610}">
   <dimension ref="A2:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -1304,7 +1371,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C96B25A2-DDD4-473B-A23E-32D8E5B261B3}">
   <dimension ref="A1:H77"/>
   <sheetViews>
-    <sheetView topLeftCell="A100" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A111" sqref="A111"/>
     </sheetView>
   </sheetViews>
@@ -1603,4 +1670,19 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A5B3C52-F9B5-4D99-B455-6FA983CD75F7}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>